<commit_message>
parent information page automation is done
</commit_message>
<xml_diff>
--- a/src/test/resources/miaPlaza.xlsx
+++ b/src/test/resources/miaPlaza.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selimoz/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selimoz/IdeaProjects/miaPlaza/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F729248E-7244-3941-8B44-DB79CBC78102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BB4FC0-9E14-6A46-856D-E18B0AC5220E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{5D842EDC-1429-9B4B-A914-6D082CA03456}"/>
+    <workbookView xWindow="40580" yWindow="2600" windowWidth="28040" windowHeight="17440" xr2:uid="{5D842EDC-1429-9B4B-A914-6D082CA03456}"/>
   </bookViews>
   <sheets>
     <sheet name="ParentInfo" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Selim</t>
   </si>
@@ -50,14 +50,38 @@
     <t>No</t>
   </si>
   <si>
-    <t>Other</t>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>option</t>
+  </si>
+  <si>
+    <t>Miacademy website,Other</t>
+  </si>
+  <si>
+    <t>siteList</t>
+  </si>
+  <si>
+    <t>startdate</t>
+  </si>
+  <si>
+    <t>07514854566</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +96,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,10 +125,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -434,44 +466,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D0ECB3-3EDD-BF42-ABDA-BF04034EC6EE}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>7514854566</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2">
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2">
         <v>45504</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{D668D749-5FE0-0548-9480-80EEC63BF771}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{D668D749-5FE0-0548-9480-80EEC63BF771}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>